<commit_message>
CotSoc added in amounts. Aggregates widget fixed
</commit_message>
<xml_diff>
--- a/data/sources/cotisations_RegimeGeneral.xlsx
+++ b/data/sources/cotisations_RegimeGeneral.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="27315" windowHeight="10260" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="20730" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="amounts" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Maladie</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>Dans tout ça, je ne sais pas s'il n'y a pas les cotisations chômage!!!</t>
+  </si>
+  <si>
+    <t>cotsoc_noncontrib</t>
+  </si>
+  <si>
+    <t>cotsoc_contrib</t>
+  </si>
+  <si>
+    <t>Attention: totaux hors non salariés</t>
   </si>
 </sst>
 </file>
@@ -735,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +845,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3">
         <v>78133000000</v>
@@ -923,7 +932,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3">
         <v>3108000000</v>
@@ -948,6 +957,64 @@
       </c>
       <c r="I7" s="3">
         <v>3576000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3">
+        <v>81241000000</v>
+      </c>
+      <c r="C8" s="3">
+        <v>83504000000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>86067000000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>89023000000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>91884000000</v>
+      </c>
+      <c r="G8" s="3">
+        <v>94363000000</v>
+      </c>
+      <c r="H8" s="3">
+        <v>94387000000</v>
+      </c>
+      <c r="I8" s="3">
+        <v>96944000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3">
+        <v>57801000000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>59527000000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>61982000000</v>
+      </c>
+      <c r="E9" s="3">
+        <v>65130000000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>66686000000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>67857000000</v>
+      </c>
+      <c r="H9" s="3">
+        <v>68049000000</v>
+      </c>
+      <c r="I9" s="3">
+        <v>69422000000</v>
       </c>
     </row>
   </sheetData>
@@ -959,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1139,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3">
         <f>B18+B38</f>
@@ -1205,7 +1272,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3">
         <f>B19+B39</f>
@@ -1272,27 +1339,81 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="1"/>
+      <c r="A9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B4+B7</f>
+        <v>81241000000</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ref="C9:I9" si="4">C4+C7</f>
+        <v>83504000000</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="4"/>
+        <v>86067000000</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="4"/>
+        <v>89023000000</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="4"/>
+        <v>91884000000</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="4"/>
+        <v>94363000000</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
+        <v>94387000000</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="4"/>
+        <v>96944000000</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
+      <c r="A10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B3+B6</f>
+        <v>57801000000</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ref="C10:I10" si="5">C3+C6</f>
+        <v>59527000000</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="5"/>
+        <v>61982000000</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="5"/>
+        <v>65130000000</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="5"/>
+        <v>66686000000</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="5"/>
+        <v>67857000000</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="5"/>
+        <v>68049000000</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="5"/>
+        <v>69422000000</v>
+      </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>